<commit_message>
doc: narrativa caso de uso paciente
</commit_message>
<xml_diff>
--- a/documentacao/TabelaTestes/TabeladeTestes_Sprint2.xlsx
+++ b/documentacao/TabelaTestes/TabeladeTestes_Sprint2.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TCC\documentacao\TabelaTestes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9B9153-6918-4FA5-8614-05CD8AC432FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -14,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
   <si>
     <t>Caso de Teste 1</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Preencher campo senha - "123456"</t>
-  </si>
-  <si>
-    <t>Preencher campo cartão do SUS - "000050069700000"</t>
   </si>
   <si>
     <t>Preencher bio - "Rinite, Sinusite, Miopia"</t>
@@ -153,7 +150,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -251,11 +248,81 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -275,21 +342,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -299,10 +372,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -582,18 +667,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D3:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,34 +691,34 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="11"/>
     </row>
@@ -642,7 +727,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="11"/>
     </row>
@@ -651,7 +736,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="11"/>
     </row>
@@ -665,29 +750,25 @@
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="2">
+      <c r="D10" s="17">
         <v>5</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="2">
-        <v>6</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="11"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <v>7</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" s="11"/>
     </row>
@@ -696,42 +777,42 @@
         <v>8</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" s="11"/>
     </row>
     <row r="14" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
     </row>
     <row r="15" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" s="11"/>
     </row>
     <row r="16" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" s="11"/>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
@@ -742,38 +823,38 @@
         <v>43910</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D26" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
+      <c r="D26" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="8"/>
+      <c r="F27" s="7"/>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <v>1</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F28" s="6"/>
     </row>
@@ -782,7 +863,7 @@
         <v>2</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F29" s="6"/>
     </row>
@@ -800,42 +881,42 @@
         <v>4</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D33" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F33" s="6"/>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D34" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F34" s="6"/>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D35" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.25">
@@ -846,38 +927,38 @@
         <v>43913</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D40" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="D40" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D41" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
+      <c r="D41" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
     </row>
     <row r="42" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D42" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="8"/>
+      <c r="F42" s="7"/>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
         <v>1</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F43" s="6"/>
     </row>
@@ -886,42 +967,42 @@
         <v>2</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F44" s="6"/>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
     </row>
     <row r="46" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D46" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F46" s="6"/>
     </row>
     <row r="47" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D47" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F47" s="6"/>
     </row>
     <row r="48" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D48" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="49" spans="4:6" x14ac:dyDescent="0.25">
@@ -932,38 +1013,38 @@
         <v>43913</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D52" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-    </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D52" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
     </row>
     <row r="53" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D53" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F53" s="8"/>
+      <c r="F53" s="7"/>
     </row>
     <row r="54" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D54" s="4">
         <v>1</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F54" s="6"/>
     </row>
@@ -972,42 +1053,42 @@
         <v>2</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F55" s="6"/>
     </row>
     <row r="56" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
     </row>
     <row r="57" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D57" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F57" s="6"/>
     </row>
     <row r="58" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D58" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F58" s="6"/>
     </row>
     <row r="59" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D59" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="60" spans="4:6" x14ac:dyDescent="0.25">
@@ -1018,38 +1099,38 @@
         <v>43922</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+    </row>
+    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D63" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-    </row>
-    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D63" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
     </row>
     <row r="64" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D64" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E64" s="8" t="s">
+      <c r="E64" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F64" s="8"/>
+      <c r="F64" s="7"/>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D65" s="4">
         <v>1</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F65" s="6"/>
     </row>
@@ -1058,42 +1139,42 @@
         <v>2</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F66" s="6"/>
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D68" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F68" s="6"/>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D69" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F69" s="6"/>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D70" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E70" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.25">
@@ -1104,39 +1185,18 @@
         <v>43915</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="D67:F67"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="D45:F45"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="D14:F14"/>
@@ -1150,13 +1210,34 @@
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:F11"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="D67:F67"/>
+    <mergeCell ref="E68:F68"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>